<commit_message>
Excel 205 to 206 Uploaded
</commit_message>
<xml_diff>
--- a/Power Query/PQ_Challenge_276.xlsx
+++ b/Power Query/PQ_Challenge_276.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgryc\Documents\excelbi_puzzles\Power Query\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB06D2D-39D7-4D23-88EC-B1BBB662AE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3B63D8-09F6-4980-8577-37DF01EAA9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,36 +253,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="5"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -406,6 +382,30 @@
           <color theme="5"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -612,18 +612,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C61218E5-22C5-4999-BCAB-D42807CC43C3}" name="input" displayName="input" ref="A1:I4" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C61218E5-22C5-4999-BCAB-D42807CC43C3}" name="input" displayName="input" ref="A1:I4" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A1:I4" xr:uid="{C61218E5-22C5-4999-BCAB-D42807CC43C3}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0EA1B8C3-6A5F-45BF-8569-DE3F294AF3E4}" name="Order ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{40E9E501-E83C-451C-9F89-88EBD7802339}" name="Shipping" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{51AC53C3-9B39-4302-812F-BF44994ECDE0}" name="Item1" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{EA96A5A8-D9DE-4915-9BB8-41595EAAACD1}" name="Qty1" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{74F1DF18-0479-4C08-8BCA-B45E213C0BFB}" name="Price1" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{BC9ACD3C-CD32-48D0-BA32-BFFF7A28102A}" name="Qty2" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{5D729F39-D131-47FD-B479-5FB5D43195B5}" name="Price2" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{CE2BBF1C-889E-4153-ABA4-F7791227DD2C}" name="Qty3" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{F9032E49-F947-4255-91BB-8CDCB6B1E7C3}" name="Price3" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{0EA1B8C3-6A5F-45BF-8569-DE3F294AF3E4}" name="Order ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{40E9E501-E83C-451C-9F89-88EBD7802339}" name="Shipping" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{51AC53C3-9B39-4302-812F-BF44994ECDE0}" name="Item1" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{EA96A5A8-D9DE-4915-9BB8-41595EAAACD1}" name="Qty1" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{74F1DF18-0479-4C08-8BCA-B45E213C0BFB}" name="Price1" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{BC9ACD3C-CD32-48D0-BA32-BFFF7A28102A}" name="Qty2" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{5D729F39-D131-47FD-B479-5FB5D43195B5}" name="Price2" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{CE2BBF1C-889E-4153-ABA4-F7791227DD2C}" name="Qty3" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{F9032E49-F947-4255-91BB-8CDCB6B1E7C3}" name="Price3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -892,7 +892,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="1171" row="5">
+  <wetp:taskpane dockstate="right" visibility="0" width="1372" row="5">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -914,6 +914,9 @@
   </we:bindings>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions val="1"/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_PYSCRIPT_CODE</we:customFunctionIds>
@@ -932,7 +935,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>